<commit_message>
Fixed UTC, PTC problem Might be worth checking any game after 9:00 PST
Also grabbed notes from betting website that are attached to the data.
</commit_message>
<xml_diff>
--- a/team_key.xlsx
+++ b/team_key.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehoffman\Documents\R\mls_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F9763311-9A42-418D-9846-692F50B3C595}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2805DF2-6098-4C8B-A0E2-C006C8C37514}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{B0BD7486-089F-4B7D-9636-CA9D802F3FC8}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
   <si>
     <t>Atlanta United FC</t>
   </si>
@@ -181,6 +181,36 @@
   </si>
   <si>
     <t>real-salt-lake</t>
+  </si>
+  <si>
+    <t>chicago-fire</t>
+  </si>
+  <si>
+    <t>colorado-rapids</t>
+  </si>
+  <si>
+    <t>columbus-crew-sc</t>
+  </si>
+  <si>
+    <t>dc-united</t>
+  </si>
+  <si>
+    <t>la-galaxy</t>
+  </si>
+  <si>
+    <t>new-york-red-bulls</t>
+  </si>
+  <si>
+    <t>san-jose-earthquakes</t>
+  </si>
+  <si>
+    <t>vancouver-whitecaps-fc</t>
+  </si>
+  <si>
+    <t>portland-timbers</t>
+  </si>
+  <si>
+    <t>philadelphia-union</t>
   </si>
 </sst>
 </file>
@@ -548,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31274E67-FD8F-4C5B-8D6A-6D08804CDC11}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +618,7 @@
         <v>47</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -598,8 +628,11 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
+      <c r="D3" t="s">
+        <v>52</v>
+      </c>
       <c r="E3">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -609,8 +642,11 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>53</v>
+      </c>
       <c r="E4">
-        <v>3</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -620,8 +656,11 @@
       <c r="C5" t="s">
         <v>32</v>
       </c>
+      <c r="D5" t="s">
+        <v>54</v>
+      </c>
       <c r="E5">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -631,8 +670,11 @@
       <c r="C6" t="s">
         <v>28</v>
       </c>
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
       <c r="E6">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -646,7 +688,7 @@
         <v>46</v>
       </c>
       <c r="E7">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -660,7 +702,7 @@
         <v>40</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -670,8 +712,11 @@
       <c r="C9" t="s">
         <v>29</v>
       </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
       <c r="E9">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -685,7 +730,7 @@
         <v>45</v>
       </c>
       <c r="E10">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -699,7 +744,7 @@
         <v>43</v>
       </c>
       <c r="E11">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -713,7 +758,7 @@
         <v>49</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -727,7 +772,7 @@
         <v>42</v>
       </c>
       <c r="E13">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -741,7 +786,7 @@
         <v>41</v>
       </c>
       <c r="E14">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -751,8 +796,11 @@
       <c r="C15" t="s">
         <v>13</v>
       </c>
+      <c r="D15" t="s">
+        <v>57</v>
+      </c>
       <c r="E15">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -766,7 +814,7 @@
         <v>48</v>
       </c>
       <c r="E16">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -776,8 +824,11 @@
       <c r="C17" t="s">
         <v>15</v>
       </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
       <c r="E17">
-        <v>16</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -787,8 +838,11 @@
       <c r="C18" t="s">
         <v>16</v>
       </c>
+      <c r="D18" t="s">
+        <v>60</v>
+      </c>
       <c r="E18">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -802,7 +856,7 @@
         <v>51</v>
       </c>
       <c r="E19">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -812,8 +866,11 @@
       <c r="C20" t="s">
         <v>18</v>
       </c>
+      <c r="D20" t="s">
+        <v>58</v>
+      </c>
       <c r="E20">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -827,7 +884,7 @@
         <v>39</v>
       </c>
       <c r="E21">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -841,7 +898,7 @@
         <v>50</v>
       </c>
       <c r="E22">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -855,7 +912,7 @@
         <v>44</v>
       </c>
       <c r="E23">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
@@ -865,8 +922,11 @@
       <c r="C24" t="s">
         <v>27</v>
       </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
       <c r="E24">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -877,7 +937,7 @@
         <v>30</v>
       </c>
       <c r="E25">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First draft of the DB is complete. Next is to add to it and clean it
</commit_message>
<xml_diff>
--- a/team_key.xlsx
+++ b/team_key.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehoffman\Documents\R\mls_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ehoff_000\Documents\R\mls_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C2805DF2-6098-4C8B-A0E2-C006C8C37514}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{B0BD7486-089F-4B7D-9636-CA9D802F3FC8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
   <si>
     <t>Atlanta United FC</t>
   </si>
@@ -211,12 +210,15 @@
   </si>
   <si>
     <t>philadelphia-union</t>
+  </si>
+  <si>
+    <t>chivas-usa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -575,11 +577,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31274E67-FD8F-4C5B-8D6A-6D08804CDC11}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -936,6 +938,9 @@
       <c r="C25" t="s">
         <v>30</v>
       </c>
+      <c r="D25" t="s">
+        <v>62</v>
+      </c>
       <c r="E25">
         <v>34</v>
       </c>

</xml_diff>

<commit_message>
Found distance between stadiums
</commit_message>
<xml_diff>
--- a/team_key.xlsx
+++ b/team_key.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="89">
   <si>
     <t>Atlanta United FC</t>
   </si>
@@ -213,13 +213,91 @@
   </si>
   <si>
     <t>chivas-usa</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>stadium</t>
+  </si>
+  <si>
+    <t>Providence Park</t>
+  </si>
+  <si>
+    <t>Mercades-Benz Arena</t>
+  </si>
+  <si>
+    <t>Toyota Park</t>
+  </si>
+  <si>
+    <t>Dick's Sporting Goods Park</t>
+  </si>
+  <si>
+    <t>MAPFRE Stadium</t>
+  </si>
+  <si>
+    <t>Audi Field</t>
+  </si>
+  <si>
+    <t>Toyota Stadium</t>
+  </si>
+  <si>
+    <t>BBVA Compass Stadium</t>
+  </si>
+  <si>
+    <t>Dignity Health Sports Park</t>
+  </si>
+  <si>
+    <t>Banc of California Stadium</t>
+  </si>
+  <si>
+    <t>Allianz Field</t>
+  </si>
+  <si>
+    <t>Saputo Stadium</t>
+  </si>
+  <si>
+    <t>Gillette Stadium</t>
+  </si>
+  <si>
+    <t>Yankee Stadium</t>
+  </si>
+  <si>
+    <t>Red Bull Arena</t>
+  </si>
+  <si>
+    <t>Orlando City Stadium</t>
+  </si>
+  <si>
+    <t>Talen Energy Stadium</t>
+  </si>
+  <si>
+    <t>Rio Tinto Stadium</t>
+  </si>
+  <si>
+    <t>Avaya Stadium</t>
+  </si>
+  <si>
+    <t>Centurylink Field</t>
+  </si>
+  <si>
+    <t>Children's Mercy Park</t>
+  </si>
+  <si>
+    <t>BMO Field</t>
+  </si>
+  <si>
+    <t>BC Palace</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +316,19 @@
       <color rgb="FF222222"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -260,10 +351,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,9 +691,12 @@
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.42578125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -608,8 +712,17 @@
       <c r="E1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,8 +735,17 @@
       <c r="E2">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="4">
+        <v>33.755428999999999</v>
+      </c>
+      <c r="H2" s="4">
+        <v>-84.401066999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -636,8 +758,17 @@
       <c r="E3">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="4">
+        <v>41.758830297999999</v>
+      </c>
+      <c r="H3" s="5">
+        <v>-87.803663451999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -650,8 +781,17 @@
       <c r="E4">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="4">
+        <v>39.805599999999998</v>
+      </c>
+      <c r="H4" s="4">
+        <v>-104.8918</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -664,8 +804,17 @@
       <c r="E5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="4">
+        <v>40.009500000000003</v>
+      </c>
+      <c r="H5" s="4">
+        <v>-82.991200000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -678,8 +827,17 @@
       <c r="E6">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="4">
+        <v>38.869</v>
+      </c>
+      <c r="H6" s="4">
+        <v>-77.012900000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -692,8 +850,17 @@
       <c r="E7">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" s="4">
+        <v>33.154299999999999</v>
+      </c>
+      <c r="H7" s="4">
+        <v>-96.8352</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -706,8 +873,17 @@
       <c r="E8">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="4">
+        <v>29.752199999999998</v>
+      </c>
+      <c r="H8" s="4">
+        <v>-95.352400000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -720,8 +896,17 @@
       <c r="E9">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>74</v>
+      </c>
+      <c r="G9" s="4">
+        <v>33.864400000000003</v>
+      </c>
+      <c r="H9" s="4">
+        <v>-118.2611</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -734,8 +919,17 @@
       <c r="E10">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>75</v>
+      </c>
+      <c r="G10" s="4">
+        <v>34.011155000000002</v>
+      </c>
+      <c r="H10" s="4">
+        <v>-117.827511</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -748,8 +942,17 @@
       <c r="E11">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F11" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="6">
+        <v>44.952778000000002</v>
+      </c>
+      <c r="H11" s="6">
+        <v>-93.165000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -762,8 +965,17 @@
       <c r="E12">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="3">
+        <v>45.5623</v>
+      </c>
+      <c r="H12" s="4">
+        <v>-73.552999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -776,8 +988,17 @@
       <c r="E13">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F13" t="s">
+        <v>78</v>
+      </c>
+      <c r="G13" s="3">
+        <v>42.090899999999998</v>
+      </c>
+      <c r="H13" s="4">
+        <v>-71.264300000000006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -790,8 +1011,17 @@
       <c r="E14">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>79</v>
+      </c>
+      <c r="G14" s="3">
+        <v>40.829599999999999</v>
+      </c>
+      <c r="H14" s="4">
+        <v>-73.926199999999994</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -804,8 +1034,17 @@
       <c r="E15">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="3">
+        <v>40.736800000000002</v>
+      </c>
+      <c r="H15" s="4">
+        <v>-74.150199999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -818,8 +1057,17 @@
       <c r="E16">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="3">
+        <v>28.5411</v>
+      </c>
+      <c r="H16" s="4">
+        <v>-81.389300000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -832,8 +1080,17 @@
       <c r="E17">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>82</v>
+      </c>
+      <c r="G17" s="3">
+        <v>39.832799999999999</v>
+      </c>
+      <c r="H17" s="4">
+        <v>-75.378500000000003</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -846,8 +1103,17 @@
       <c r="E18">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F18" t="s">
+        <v>66</v>
+      </c>
+      <c r="G18" s="4">
+        <v>45.521500000000003</v>
+      </c>
+      <c r="H18" s="5">
+        <v>-122.6918</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -860,8 +1126,17 @@
       <c r="E19">
         <v>28</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F19" t="s">
+        <v>83</v>
+      </c>
+      <c r="G19" s="3">
+        <v>40.582900000000002</v>
+      </c>
+      <c r="H19" s="4">
+        <v>-111.8934</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -874,8 +1149,17 @@
       <c r="E20">
         <v>29</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>84</v>
+      </c>
+      <c r="G20" s="3">
+        <v>37.351100000000002</v>
+      </c>
+      <c r="H20" s="4">
+        <v>-121.9246</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -888,8 +1172,17 @@
       <c r="E21">
         <v>30</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F21" t="s">
+        <v>85</v>
+      </c>
+      <c r="G21" s="3">
+        <v>47.595199999999998</v>
+      </c>
+      <c r="H21" s="4">
+        <v>-122.33159999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -902,8 +1195,17 @@
       <c r="E22">
         <v>31</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F22" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="3">
+        <v>39.121600000000001</v>
+      </c>
+      <c r="H22" s="4">
+        <v>-94.8232</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -916,8 +1218,17 @@
       <c r="E23">
         <v>32</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="3">
+        <v>43.633200000000002</v>
+      </c>
+      <c r="H23" s="4">
+        <v>-79.418599999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -930,8 +1241,17 @@
       <c r="E24">
         <v>33</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" t="s">
+        <v>88</v>
+      </c>
+      <c r="G24" s="3">
+        <v>49.276800000000001</v>
+      </c>
+      <c r="H24" s="4">
+        <v>-123.11199999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>26</v>
       </c>
@@ -943,6 +1263,15 @@
       </c>
       <c r="E25">
         <v>34</v>
+      </c>
+      <c r="F25" t="s">
+        <v>74</v>
+      </c>
+      <c r="G25" s="4">
+        <v>33.864400000000003</v>
+      </c>
+      <c r="H25" s="4">
+        <v>-118.2611</v>
       </c>
     </row>
   </sheetData>

</xml_diff>